<commit_message>
Limit Management Slider Update work
</commit_message>
<xml_diff>
--- a/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/ChangeLoginPassword.xlsx
+++ b/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/ChangeLoginPassword.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HBL-Automation-852020-ETDR\HBLAutomationWeb\Resources\Feature\InternetBanking\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HBL-Automation-8262020\HBLAutomationWeb\Resources\Feature\InternetBanking\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Case</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Select STATUS FROM DC_TRANSACTION DT WHERE DT.CHANNEL_ID='2'and  DT.TRANSACTION_ID = '</t>
+  </si>
+  <si>
+    <t>customer_password_query</t>
+  </si>
+  <si>
+    <t>Select count(*) from (Select MAX(AA.CREATED_ON) from DC_CUSTOMER_PASSWORD_HISTORY AA INNER JOIN DC_CUSTOMER_INFO BB ON AA.CUSTOMER_INFO_ID = BB.CUSTOMER_INFO_ID where AA.CUSTOMER_INFO_ID = (Select CUSTOMER_INFO_ID from dc_customer_info l where L.CUSTOMER_NAME = '{customer_name}') and AA.TRANSACTION_TYPE_ID = (Select LL.TRANSACTION_TYPE_ID from DC_TRANSACTION LL where LL.TRANSACTION_ID = '{TRANSACTION_ID}') and AA.PASSWORD = BB.LOGIN_PASSWORD and TRUNC(AA.CREATED_ON) &lt; (SELECT TRUNC(SYSDATE) FROM DUAL) and TRUNC(AA.UPDATED_ON) &lt; (SELECT TRUNC(SYSDATE) FROM DUAL) order by AA.UPDATED_ON desc) where rownum = 1</t>
   </si>
 </sst>
 </file>
@@ -442,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,11 +470,12 @@
     <col min="14" max="14" width="185.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="102.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="9.140625" style="3"/>
+    <col min="18" max="18" width="255.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" style="3"/>
     <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,8 +527,11 @@
       <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="R1" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -572,6 +582,9 @@
       </c>
       <c r="Q2" s="3" t="s">
         <v>26</v>
+      </c>
+      <c r="R2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>